<commit_message>
Updated Team Member's Job's Specification
</commit_message>
<xml_diff>
--- a/TeamMembersJobsSpecification.xlsx
+++ b/TeamMembersJobsSpecification.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Music\Applied-Project-4th-Year\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Project Spec:</t>
   </si>
@@ -42,9 +47,6 @@
     <t>3 Games (Problem-Solving)</t>
   </si>
   <si>
-    <t>1 Game (Memory)</t>
-  </si>
-  <si>
     <t>Github:</t>
   </si>
   <si>
@@ -54,9 +56,6 @@
     <t>Team Members:</t>
   </si>
   <si>
-    <t>Master</t>
-  </si>
-  <si>
     <t>Host Website on Azure</t>
   </si>
   <si>
@@ -78,9 +77,6 @@
     <t>Aquire sounds and incorporate these into the application</t>
   </si>
   <si>
-    <t>Get list of users signed up to website displayed in-app using JSON GET Request</t>
-  </si>
-  <si>
     <t>Ensure Main-Page is structured/navigates to all paths specified in buttons</t>
   </si>
   <si>
@@ -96,25 +92,55 @@
     <t>Thesis</t>
   </si>
   <si>
-    <t>Methodology Section</t>
-  </si>
-  <si>
-    <t>System Evaluation section</t>
-  </si>
-  <si>
-    <t>Introduction Section</t>
-  </si>
-  <si>
     <t>Write about above in Technology Review</t>
   </si>
   <si>
-    <t>System Design Section</t>
+    <t>Master (Upload all team member's work due to merge conflicts)</t>
+  </si>
+  <si>
+    <t>Get list of users signed up to website displayed in-app using SlashDB API</t>
+  </si>
+  <si>
+    <t>System Evaluation section/Testing/Requirements</t>
+  </si>
+  <si>
+    <t>Methodology Section explaining Agile as preferred methodology</t>
+  </si>
+  <si>
+    <t>Introduction Section/Table of Contents &amp; Figures generation</t>
+  </si>
+  <si>
+    <t>System Design Section with Architechture of project</t>
+  </si>
+  <si>
+    <t>2 Games (Memory)</t>
+  </si>
+  <si>
+    <t>Input on all sections referencing above jobs</t>
+  </si>
+  <si>
+    <t>Proof-read thesis, correct grammatical errors/unreadable sentences</t>
+  </si>
+  <si>
+    <t>Referencing</t>
+  </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
+  <si>
+    <t>ScreenCast of entire project using ShareX</t>
+  </si>
+  <si>
+    <t>Associating app with Windows store/Testing using App Cert Kit</t>
+  </si>
+  <si>
+    <t>Selenium Test Suit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,8 +170,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -158,6 +187,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -206,7 +238,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,9 +271,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -274,6 +323,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -450,35 +516,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" customWidth="1"/>
+    <col min="2" max="2" width="60.28515625" customWidth="1"/>
     <col min="3" max="3" width="71" customWidth="1"/>
-    <col min="4" max="4" width="50.42578125" customWidth="1"/>
+    <col min="4" max="4" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -495,30 +561,30 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -532,103 +598,152 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>